<commit_message>
Definición de costos - Release Planning
#53 Se actualiza el Release Planning y se agregan los costos sobre cada avión.
</commit_message>
<xml_diff>
--- a/release planning.xlsx
+++ b/release planning.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Universidad\5to Semestre\Ejercicio Naves de papel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmontanez\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Historias - Documentadas" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Historias - Documentadas'!$B$2:$F$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="42">
   <si>
     <t>HISTORIAS</t>
   </si>
@@ -124,14 +124,48 @@
   </si>
   <si>
     <t>TIEMPO (Min)</t>
+  </si>
+  <si>
+    <t>Desarrollo</t>
+  </si>
+  <si>
+    <t>Análisis</t>
+  </si>
+  <si>
+    <t>Diseño</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>1 Avion mediano</t>
+  </si>
+  <si>
+    <t>1 Avion grande</t>
+  </si>
+  <si>
+    <t>1 Avion Pequeño</t>
+  </si>
+  <si>
+    <t>1 Avion mediano color</t>
+  </si>
+  <si>
+    <t>1 Avion pequeño color</t>
+  </si>
+  <si>
+    <t>1 Avion mediano diseño</t>
+  </si>
+  <si>
+    <t>1 Avion pequeño diseño</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;\ * #,##0.00_);_(&quot;$&quot;\ * \(#,##0.00\);_(&quot;$&quot;\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -385,11 +419,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -429,27 +464,29 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Moneda" xfId="1" builtinId="4"/>
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="2" builtinId="7"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,24 +765,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K17"/>
+  <dimension ref="B2:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" style="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.44140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
@@ -762,7 +799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>23</v>
       </c>
@@ -783,7 +820,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -804,7 +841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
@@ -825,7 +862,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
@@ -846,7 +883,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
@@ -867,7 +904,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
@@ -888,7 +925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>19</v>
       </c>
@@ -909,7 +946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>20</v>
       </c>
@@ -927,19 +964,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="14">
         <v>3</v>
       </c>
       <c r="E11" s="23">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>4</v>
@@ -948,7 +985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
@@ -969,20 +1006,190 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>34</v>
+      </c>
       <c r="I15" s="17"/>
       <c r="J15" s="17"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="1">
+        <f>$C$10/3</f>
+        <v>5</v>
+      </c>
+      <c r="D16" s="1">
+        <f>$C$3/9 + $C$5/9 + $C$6/9 + $C$7/9</f>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E16" s="1">
+        <f>$C$4/9</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F16" s="31">
+        <f>ROUNDUP(SUM(C16:E16),0)</f>
+        <v>14</v>
+      </c>
       <c r="I16" s="17"/>
       <c r="J16" s="17"/>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="1">
+        <f>$C$9/3</f>
+        <v>5</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" ref="D17:D22" si="1">$C$3/9 + $C$5/9 + $C$6/9 + $C$7/9</f>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" ref="E17:E20" si="2">$C$4/9</f>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F17" s="31">
+        <f>ROUNDUP(SUM(C17:E17),0)</f>
+        <v>14</v>
+      </c>
       <c r="I17" s="17"/>
       <c r="J17" s="17"/>
       <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1">
+        <f>$C$8/3</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="F18" s="31">
+        <f>ROUNDUP(SUM(C18:E18),0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="1">
+        <f>$C$11/3</f>
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E19" s="1">
+        <f>$C$4/9 + $C$11/9</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="F19" s="31">
+        <f>ROUNDUP(SUM(C19:E19),0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="1">
+        <f>$C$11/3</f>
+        <v>2</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E20" s="1">
+        <f>$C$4/9 + $C$12/9</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="F20" s="31">
+        <f>ROUNDUP(SUM(C20:E20),0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="1">
+        <f t="shared" ref="C21:C22" si="3">$C$8/3</f>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E21" s="1">
+        <f>$C$4/9 + $C$11/9</f>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="F21" s="31">
+        <f>ROUNDUP(SUM(C21:E21),0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="1">
+        <f t="shared" si="3"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="E22" s="1">
+        <f>$C$4/9 + $C$12/9</f>
+        <v>2.2222222222222223</v>
+      </c>
+      <c r="F22" s="31">
+        <f>ROUNDUP(SUM(C22:E22),0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="F27" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="B2:F12">
@@ -999,137 +1206,137 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="22" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="30" t="s">
+    <row r="1" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D2" s="27" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="19"/>
     </row>
-    <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="27"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="27"/>
-    </row>
-    <row r="6" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" s="30"/>
+    </row>
+    <row r="7" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="28" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="27"/>
-    </row>
-    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="27"/>
-    </row>
-    <row r="10" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="28" t="s">
+      <c r="E9" s="29"/>
+    </row>
+    <row r="10" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="29"/>
-    </row>
-    <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="30"/>
+    </row>
+    <row r="11" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="28" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="29"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="28" t="s">
+    <row r="13" spans="2:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="29"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E14" s="20"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E15" s="20"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="E16" s="21"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
       <c r="E17" s="21"/>
       <c r="F17" s="3"/>
     </row>

</xml_diff>